<commit_message>
updated contents and readme
</commit_message>
<xml_diff>
--- a/contents.xlsx
+++ b/contents.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
   <si>
     <t xml:space="preserve">Subject</t>
   </si>
@@ -67,9 +67,6 @@
     <t xml:space="preserve">Age distribution</t>
   </si>
   <si>
-    <t xml:space="preserve">Stratified by sex; need to combine male (003-025) and female (027-049)</t>
-  </si>
-  <si>
     <t xml:space="preserve">026</t>
   </si>
   <si>
@@ -88,7 +85,7 @@
     <t xml:space="preserve">pct_*</t>
   </si>
   <si>
-    <t xml:space="preserve">Racial composition - black nonhisp, white nonhisp, asian nonhisp, hispanic, two or more</t>
+    <t xml:space="preserve">Racial composition by percentage - black nonhisp, white nonhisp, asian nonhisp, hispanic, two or more</t>
   </si>
   <si>
     <t xml:space="preserve">B08301</t>
@@ -136,7 +133,7 @@
     <t xml:space="preserve">pct_poverty</t>
   </si>
   <si>
-    <t xml:space="preserve">S</t>
+    <t xml:space="preserve">Percent below poverty level</t>
   </si>
   <si>
     <t xml:space="preserve">B19013</t>
@@ -184,7 +181,7 @@
     <t xml:space="preserve">Unemployment rate (for age 16 and over)</t>
   </si>
   <si>
-    <t xml:space="preserve">not available 2009-2010</t>
+    <t xml:space="preserve">Not available 2009-2010</t>
   </si>
   <si>
     <t xml:space="preserve">B25008</t>
@@ -217,10 +214,19 @@
     <t xml:space="preserve">Median property value</t>
   </si>
   <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">population_density</t>
   </si>
   <si>
     <t xml:space="preserve">Population density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TODO: calculate after spatial join</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIP</t>
   </si>
 </sst>
 </file>
@@ -341,16 +347,16 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="44.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="58.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -403,9 +409,6 @@
       <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" s="0" t="s">
         <v>10</v>
       </c>
@@ -415,13 +418,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>10</v>
@@ -429,16 +432,16 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>10</v>
@@ -446,16 +449,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>10</v>
@@ -463,16 +466,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>10</v>
@@ -480,16 +483,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>10</v>
@@ -497,16 +500,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>10</v>
@@ -514,19 +517,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>10</v>
@@ -534,16 +537,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="D11" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>10</v>
@@ -551,19 +554,19 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="E12" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>10</v>
@@ -571,19 +574,19 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>10</v>
@@ -591,16 +594,16 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="D14" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>10</v>
@@ -608,16 +611,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>10</v>
@@ -625,30 +628,42 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="C17" s="0" t="s">
         <v>64</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>65</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added extra race variables
</commit_message>
<xml_diff>
--- a/contents.xlsx
+++ b/contents.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
   <si>
     <t xml:space="preserve">Subject</t>
   </si>
@@ -76,16 +76,25 @@
     <t xml:space="preserve">Percent female</t>
   </si>
   <si>
+    <t xml:space="preserve">B02001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">002,003,005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pct_*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Race composition – white, black, asian</t>
+  </si>
+  <si>
     <t xml:space="preserve">B03002</t>
   </si>
   <si>
-    <t xml:space="preserve">003,004,006,012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pct_*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Racial composition by percentage - black nonhisp, white nonhisp, asian nonhisp, hispanic, two or more</t>
+    <t xml:space="preserve">003,004,006,013,014,016,012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Race composition by percentage with hispanic + latino origin separated - black nonhisp, white nonhisp, asian nonhisp, hispanic, two or more</t>
   </si>
   <si>
     <t xml:space="preserve">B08301</t>
@@ -344,19 +353,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="58.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.97"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,10 +464,10 @@
         <v>22</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>10</v>
@@ -466,16 +475,16 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>10</v>
@@ -483,16 +492,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>10</v>
@@ -500,16 +509,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>10</v>
@@ -517,10 +526,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>38</v>
@@ -528,25 +537,25 @@
       <c r="D10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="F10" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="E11" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>10</v>
@@ -554,19 +563,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>46</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>40</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>10</v>
@@ -577,16 +583,16 @@
         <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="D13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E13" s="0" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>10</v>
@@ -594,15 +600,18 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="D14" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="0" t="s">
         <v>55</v>
       </c>
       <c r="F14" s="0" t="s">
@@ -614,24 +623,24 @@
         <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="F15" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>61</v>
@@ -639,19 +648,16 @@
       <c r="D16" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="F16" s="0" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="0" t="s">
         <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>64</v>
@@ -660,10 +666,30 @@
         <v>65</v>
       </c>
       <c r="E17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="B18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>67</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
decennial census variables draft
</commit_message>
<xml_diff>
--- a/contents.xlsx
+++ b/contents.xlsx
@@ -23,12 +23,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
-  <si>
-    <t xml:space="preserve">Subject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tables</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="96">
+  <si>
+    <t xml:space="preserve">ACS subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACS tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decennial subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decennial tables</t>
   </si>
   <si>
     <t xml:space="preserve">Generated variable</t>
@@ -40,7 +46,10 @@
     <t xml:space="preserve">Note</t>
   </si>
   <si>
-    <t xml:space="preserve">Added</t>
+    <t xml:space="preserve">Added ACS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Decennial</t>
   </si>
   <si>
     <t xml:space="preserve">B01001</t>
@@ -49,6 +58,12 @@
     <t xml:space="preserve">001</t>
   </si>
   <si>
+    <t xml:space="preserve">P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P0010001</t>
+  </si>
+  <si>
     <t xml:space="preserve">population</t>
   </si>
   <si>
@@ -61,6 +76,12 @@
     <t xml:space="preserve">003-025,027-049</t>
   </si>
   <si>
+    <t xml:space="preserve">P12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P0120003-P0120025,P0120027-P0120049</t>
+  </si>
+  <si>
     <t xml:space="preserve">pct_age_*</t>
   </si>
   <si>
@@ -70,6 +91,9 @@
     <t xml:space="preserve">026</t>
   </si>
   <si>
+    <t xml:space="preserve">P0120026</t>
+  </si>
+  <si>
     <t xml:space="preserve">pct_female</t>
   </si>
   <si>
@@ -82,6 +106,12 @@
     <t xml:space="preserve">002,003,005</t>
   </si>
   <si>
+    <t xml:space="preserve">P3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P0030002,P0030003,P0030005</t>
+  </si>
+  <si>
     <t xml:space="preserve">pct_*</t>
   </si>
   <si>
@@ -94,6 +124,12 @@
     <t xml:space="preserve">003,004,006,013,014,016,012</t>
   </si>
   <si>
+    <t xml:space="preserve">P5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P0050003,P0050004,P0050006P0050011,P0050012,P0050014,P0050010</t>
+  </si>
+  <si>
     <t xml:space="preserve">Race composition by percentage with hispanic + latino origin separated - black nonhisp, white nonhisp, asian nonhisp, hispanic, two or more</t>
   </si>
   <si>
@@ -103,6 +139,9 @@
     <t xml:space="preserve">002,010-021</t>
   </si>
   <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">pct_transport_*</t>
   </si>
   <si>
@@ -196,6 +235,12 @@
     <t xml:space="preserve">B25008</t>
   </si>
   <si>
+    <t xml:space="preserve">H11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H0110004</t>
+  </si>
+  <si>
     <t xml:space="preserve">pct_renting</t>
   </si>
   <si>
@@ -223,19 +268,49 @@
     <t xml:space="preserve">Median property value</t>
   </si>
   <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
     <t xml:space="preserve">population_density</t>
   </si>
   <si>
     <t xml:space="preserve">Population density</t>
   </si>
   <si>
-    <t xml:space="preserve">TODO: calculate after spatial join</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WIP</t>
+    <t xml:space="preserve">Not included; use spatial join</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B19083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gini_index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gini index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P0050001,P0050003,P0050004,P0050006,P0050010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ethnic_fractionalization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethnic fractionalization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See inputs/B19001_cutoffs.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ice_income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index of Concentration at the Extremes for income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P0050001,P0050003,P0050004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ice_race_ethnicity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index of Concentration at the Extremes for race / ethnicity</t>
   </si>
 </sst>
 </file>
@@ -345,6 +420,100 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFCC0000"/>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF006600"/>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -353,19 +522,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="58.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="50.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.97"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,324 +544,594 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>10</v>
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>10</v>
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>10</v>
+        <v>42</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>10</v>
+        <v>46</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>10</v>
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>42</v>
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>10</v>
+        <v>54</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>10</v>
+        <v>58</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>50</v>
+        <v>10</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>10</v>
+        <v>62</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>54</v>
+        <v>65</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>10</v>
+        <v>66</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>10</v>
+      <c r="C15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>10</v>
+        <v>75</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>65</v>
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>10</v>
+        <v>79</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>68</v>
+        <v>38</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>70</v>
+        <v>81</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>1003004</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C1:D1048576">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"NA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:I1048576">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"NA"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
added variables for heating; fixed percentages of housing types
</commit_message>
<xml_diff>
--- a/contents.xlsx
+++ b/contents.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="100">
   <si>
     <t xml:space="preserve">ACS subject</t>
   </si>
@@ -257,6 +257,18 @@
   </si>
   <si>
     <t xml:space="preserve">Housing units per building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B25040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">002-010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pct_heating_*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of heating</t>
   </si>
   <si>
     <t xml:space="preserve">B25077</t>
@@ -522,18 +534,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="50.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="50.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.97"/>
   </cols>
   <sheetData>
@@ -562,7 +574,7 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -588,7 +600,7 @@
       <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -637,7 +649,7 @@
       <c r="H4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -663,7 +675,7 @@
       <c r="H5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -689,7 +701,7 @@
       <c r="H6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -715,7 +727,7 @@
       <c r="H7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -741,7 +753,7 @@
       <c r="H8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -767,7 +779,7 @@
       <c r="H9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -793,7 +805,7 @@
       <c r="H10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="I10" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -822,7 +834,7 @@
       <c r="H11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -848,7 +860,7 @@
       <c r="H12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -877,7 +889,7 @@
       <c r="H13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -906,7 +918,7 @@
       <c r="H14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="I14" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -932,7 +944,7 @@
       <c r="H15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="I15" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -958,163 +970,189 @@
       <c r="H16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G17" s="0" t="s">
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>83</v>
-      </c>
       <c r="H18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F19" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="H21" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="0" t="s">
+      <c r="G19" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>87</v>
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>15</v>
+        <v>90</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>90</v>
+        <v>33</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>38</v>
+        <v>93</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B25" s="0" t="n">
         <v>1003004</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="0" t="s">
+      <c r="D25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>